<commit_message>
updated checklist, renamed file
</commit_message>
<xml_diff>
--- a/Custom-OWASP-Checklist-Phase4.xlsx
+++ b/Custom-OWASP-Checklist-Phase4.xlsx
@@ -24,6 +24,202 @@
     <author>Thomas</author>
   </authors>
   <commentList>
+    <comment ref="D6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Team7 BB Chapter 3.6</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>BB Team4 Chapter 3.2</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Slide 24</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">BB Team4 Chapter 3.6
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>slide 35</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">BB Team4 Chapter 3.5
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>slide 33</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E35" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">BB Team4 Chapter 3.1
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F35" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>slide 20</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E39" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">BB Team4 Chapter 3.3
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F39" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>slide 26</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E42" authorId="0">
       <text>
         <r>
@@ -37,7 +233,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D47" authorId="0">
+    <comment ref="F42" authorId="0">
       <text>
         <r>
           <rPr>
@@ -46,7 +242,7 @@
             <color indexed="81"/>
             <rFont val="Arial"/>
           </rPr>
-          <t>BB Chapter 4.1</t>
+          <t>Slide 30</t>
         </r>
         <r>
           <rPr>
@@ -68,7 +264,29 @@
             <color indexed="81"/>
             <rFont val="Arial"/>
           </rPr>
-          <t xml:space="preserve">BB Chapter 4.2
+          <t>BB Chapter 4.1.6</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E48" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">BB Team4 Chapter 3.1
 </t>
         </r>
         <r>
@@ -78,6 +296,32 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F48" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">slide 26
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D49" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">BB Team 7 Chapter 4.2.6
 </t>
         </r>
       </text>
@@ -95,7 +339,46 @@
         </r>
       </text>
     </comment>
+    <comment ref="E52" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>BB Team 4 Chapter 3.7.2</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D53" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>BB: Chapter 5.1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D60" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>BB: Chapter 5.3.6</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E60" authorId="0">
       <text>
         <r>
           <rPr>
@@ -113,7 +396,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="264">
   <si>
     <t>Ref. No.</t>
   </si>
@@ -997,7 +1280,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1023,8 +1306,88 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1058,15 +1421,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="105">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -1079,6 +1439,46 @@
     <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="104" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -1091,6 +1491,46 @@
     <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="103" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1479,8 +1919,8 @@
   <dimension ref="A1:Z980"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1491,7 +1931,7 @@
     <col min="4" max="4" width="20.83203125" customWidth="1"/>
     <col min="5" max="5" width="17.33203125" customWidth="1"/>
     <col min="6" max="6" width="9.5" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="24.75" customHeight="1">
@@ -1594,9 +2034,15 @@
       <c r="C6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="4"/>
+      <c r="D6" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>28</v>
+      </c>
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:26" ht="12">
@@ -1639,9 +2085,15 @@
       <c r="C9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="8"/>
+      <c r="D9" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>28</v>
+      </c>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:26" ht="12">
@@ -1657,9 +2109,13 @@
       <c r="D10" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="5"/>
+      <c r="E10" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="F10" s="4"/>
-      <c r="G10" s="5"/>
+      <c r="G10" s="10" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="12">
       <c r="D11" s="4"/>
@@ -1689,9 +2145,7 @@
       <c r="C13" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>40</v>
-      </c>
+      <c r="D13" s="8"/>
       <c r="E13" s="5"/>
       <c r="F13" s="4"/>
       <c r="G13" s="5"/>
@@ -1816,9 +2270,15 @@
       <c r="C22" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="4"/>
+      <c r="D22" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>28</v>
+      </c>
       <c r="G22" s="5"/>
     </row>
     <row r="23" spans="1:7" ht="12">
@@ -1876,9 +2336,7 @@
       <c r="C26" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D26" s="9" t="s">
-        <v>40</v>
-      </c>
+      <c r="D26" s="8"/>
       <c r="E26" s="5"/>
       <c r="F26" s="4"/>
       <c r="G26" s="5"/>
@@ -1896,9 +2354,13 @@
       <c r="D27" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E27" s="5"/>
+      <c r="E27" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="F27" s="4"/>
-      <c r="G27" s="5"/>
+      <c r="G27" s="10" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="12">
       <c r="A28" s="6" t="s">
@@ -1913,9 +2375,13 @@
       <c r="D28" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E28" s="5"/>
+      <c r="E28" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="F28" s="4"/>
-      <c r="G28" s="5"/>
+      <c r="G28" s="10" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="12">
       <c r="A29" s="6" t="s">
@@ -2005,9 +2471,15 @@
       <c r="C35" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="4"/>
+      <c r="D35" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="G35" s="5"/>
     </row>
     <row r="36" spans="1:7" ht="12">
@@ -2053,9 +2525,15 @@
       <c r="C39" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="D39" s="4"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="4"/>
+      <c r="D39" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="G39" s="5"/>
     </row>
     <row r="40" spans="1:7" ht="12">
@@ -2098,7 +2576,9 @@
       <c r="C42" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="D42" s="4"/>
+      <c r="D42" s="14" t="s">
+        <v>11</v>
+      </c>
       <c r="E42" s="12" t="s">
         <v>263</v>
       </c>
@@ -2165,11 +2645,6 @@
       <c r="C47" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="D47" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="E47" s="5"/>
-      <c r="F47" s="4"/>
       <c r="G47" s="5"/>
     </row>
     <row r="48" spans="1:7" ht="12">
@@ -2203,7 +2678,9 @@
       <c r="C49" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="D49" s="4"/>
+      <c r="D49" s="11" t="s">
+        <v>262</v>
+      </c>
       <c r="E49" s="5"/>
       <c r="F49" s="4"/>
       <c r="G49" s="5"/>
@@ -2221,9 +2698,13 @@
       <c r="D50" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E50" s="5"/>
+      <c r="E50" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="F50" s="4"/>
-      <c r="G50" s="5"/>
+      <c r="G50" s="10" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="51" spans="1:7" ht="12">
       <c r="A51" s="6" t="s">
@@ -2244,16 +2725,18 @@
       <c r="A52" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="B52" s="14" t="s">
+      <c r="B52" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="C52" s="14" t="s">
+      <c r="C52" s="13" t="s">
         <v>134</v>
       </c>
       <c r="D52" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E52" s="5"/>
+      <c r="E52" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="F52" s="4"/>
       <c r="G52" s="5"/>
     </row>
@@ -2284,9 +2767,13 @@
       <c r="D54" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E54" s="5"/>
+      <c r="E54" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="F54" s="4"/>
-      <c r="G54" s="5"/>
+      <c r="G54" s="10" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="55" spans="1:7" ht="12">
       <c r="A55" s="6" t="s">
@@ -2301,9 +2788,13 @@
       <c r="D55" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E55" s="5"/>
+      <c r="E55" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="F55" s="4"/>
-      <c r="G55" s="5"/>
+      <c r="G55" s="10" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="56" spans="1:7" ht="12">
       <c r="A56" s="6" t="s">
@@ -2315,10 +2806,16 @@
       <c r="C56" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="D56" s="4"/>
-      <c r="E56" s="5"/>
+      <c r="D56" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="F56" s="4"/>
-      <c r="G56" s="5"/>
+      <c r="G56" s="10" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="57" spans="1:7" ht="12">
       <c r="A57" s="6" t="s">
@@ -2333,9 +2830,13 @@
       <c r="D57" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E57" s="5"/>
+      <c r="E57" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="F57" s="4"/>
-      <c r="G57" s="5"/>
+      <c r="G57" s="10" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="58" spans="1:7" ht="12">
       <c r="A58" s="6" t="s">
@@ -2350,9 +2851,13 @@
       <c r="D58" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E58" s="5"/>
+      <c r="E58" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="F58" s="4"/>
-      <c r="G58" s="5"/>
+      <c r="G58" s="10" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="59" spans="1:7" ht="12">
       <c r="A59" s="6" t="s">
@@ -2367,9 +2872,13 @@
       <c r="D59" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E59" s="5"/>
+      <c r="E59" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="F59" s="4"/>
-      <c r="G59" s="5"/>
+      <c r="G59" s="10" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="60" spans="1:7" ht="12">
       <c r="A60" s="6" t="s">
@@ -2381,8 +2890,12 @@
       <c r="C60" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="D60" s="4"/>
-      <c r="E60" s="5"/>
+      <c r="D60" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E60" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="F60" s="4"/>
       <c r="G60" s="5"/>
     </row>
@@ -2435,8 +2948,12 @@
       <c r="C64" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="D64" s="13"/>
-      <c r="E64" s="5"/>
+      <c r="D64" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E64" s="14" t="s">
+        <v>11</v>
+      </c>
       <c r="F64" s="4"/>
       <c r="G64" s="5"/>
     </row>
@@ -2447,8 +2964,12 @@
       <c r="C65" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="D65" s="13"/>
-      <c r="E65" s="5"/>
+      <c r="D65" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E65" s="14" t="s">
+        <v>11</v>
+      </c>
       <c r="F65" s="4"/>
       <c r="G65" s="5"/>
     </row>
@@ -2459,8 +2980,12 @@
       <c r="C66" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="D66" s="4"/>
-      <c r="E66" s="5"/>
+      <c r="D66" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E66" s="14" t="s">
+        <v>11</v>
+      </c>
       <c r="F66" s="4"/>
       <c r="G66" s="5"/>
     </row>
@@ -2471,8 +2996,12 @@
       <c r="C67" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="D67" s="4"/>
-      <c r="E67" s="5"/>
+      <c r="D67" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E67" s="14" t="s">
+        <v>11</v>
+      </c>
       <c r="F67" s="4"/>
       <c r="G67" s="5"/>
     </row>
@@ -2480,7 +3009,7 @@
       <c r="A68" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B68" s="6" t="s">
+      <c r="B68" s="13" t="s">
         <v>175</v>
       </c>
       <c r="C68" s="6" t="s">
@@ -2501,7 +3030,7 @@
       <c r="C69" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="D69" s="15" t="s">
+      <c r="D69" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E69" s="5"/>
@@ -2602,9 +3131,13 @@
       <c r="D77" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E77" s="5"/>
+      <c r="E77" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="F77" s="4"/>
-      <c r="G77" s="5"/>
+      <c r="G77" s="10" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="78" spans="1:7" ht="12">
       <c r="A78" s="6" t="s">
@@ -2649,9 +3182,7 @@
       <c r="C81" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="D81" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="D81" s="8"/>
       <c r="E81" s="5"/>
       <c r="F81" s="4"/>
       <c r="G81" s="5"/>
@@ -2696,8 +3227,12 @@
       <c r="C84" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="D84" s="4"/>
-      <c r="E84" s="5"/>
+      <c r="D84" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E84" s="14" t="s">
+        <v>11</v>
+      </c>
       <c r="F84" s="4"/>
       <c r="G84" s="12" t="s">
         <v>27</v>
@@ -2851,7 +3386,7 @@
       <c r="C95" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="D95" s="15" t="s">
+      <c r="D95" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E95" s="5"/>
@@ -2868,7 +3403,7 @@
       <c r="C96" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="D96" s="15" t="s">
+      <c r="D96" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E96" s="5"/>
@@ -8254,6 +8789,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <extLst>

</xml_diff>